<commit_message>
Updated excel with input
</commit_message>
<xml_diff>
--- a/InputData.xlsx
+++ b/InputData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nirmal\Documents\UiPath\UnityBrokers_Dispatcher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB17AD2-7E6E-4B7E-9D90-D4FDFCABC39C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C273B35-B819-4A23-86E8-BA238D5464C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>Email</t>
   </si>
@@ -109,6 +109,60 @@
   </si>
   <si>
     <t>Previous policy expiry</t>
+  </si>
+  <si>
+    <t>INDIVIDUAL</t>
+  </si>
+  <si>
+    <t>YADHUKRISHNAN</t>
+  </si>
+  <si>
+    <t>yadhutest@gmail.com</t>
+  </si>
+  <si>
+    <t>United Arab Emirates</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>JN8AY2NY3F9133738</t>
+  </si>
+  <si>
+    <t>19/08/2015</t>
+  </si>
+  <si>
+    <t>Abu Dhabi</t>
+  </si>
+  <si>
+    <t>21/04/2002</t>
+  </si>
+  <si>
+    <t>0 Year</t>
+  </si>
+  <si>
+    <t>Motor Comprehensive</t>
+  </si>
+  <si>
+    <t>1974-7959051-1</t>
+  </si>
+  <si>
+    <t>18/04/2032</t>
+  </si>
+  <si>
+    <t>ABU DHABI</t>
+  </si>
+  <si>
+    <t>Salaried (Private Sector)</t>
+  </si>
+  <si>
+    <t>WHITE</t>
+  </si>
+  <si>
+    <t>VK5600798P</t>
+  </si>
+  <si>
+    <t>21/11/2025</t>
   </si>
 </sst>
 </file>
@@ -153,9 +207,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -439,21 +494,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="AB1" sqref="AB1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
@@ -463,6 +518,17 @@
     <col min="16" max="16" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -552,9 +618,86 @@
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2">
+        <v>508037025</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="2">
+        <v>36321</v>
+      </c>
+      <c r="G2">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" t="s">
+        <v>37</v>
+      </c>
+      <c r="R2" t="s">
+        <v>38</v>
+      </c>
+      <c r="S2" t="s">
+        <v>39</v>
+      </c>
+      <c r="T2">
+        <v>401011</v>
+      </c>
+      <c r="U2" t="s">
+        <v>40</v>
+      </c>
+      <c r="V2" t="s">
+        <v>41</v>
+      </c>
+      <c r="W2" t="s">
+        <v>42</v>
+      </c>
+      <c r="X2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y2">
+        <v>1980269076</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{7B264015-19CD-4504-AF81-4D7A9D45016E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated with latest changes - 02/12/2025
</commit_message>
<xml_diff>
--- a/InputData.xlsx
+++ b/InputData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nirmal\Documents\UiPath\UnityBrokers_Dispatcher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C273B35-B819-4A23-86E8-BA238D5464C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B43499A-5A72-441D-AC93-8B16BABC8DF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
   <si>
     <t>Email</t>
   </si>
@@ -114,9 +114,6 @@
     <t>INDIVIDUAL</t>
   </si>
   <si>
-    <t>YADHUKRISHNAN</t>
-  </si>
-  <si>
     <t>yadhutest@gmail.com</t>
   </si>
   <si>
@@ -163,6 +160,12 @@
   </si>
   <si>
     <t>21/11/2025</t>
+  </si>
+  <si>
+    <t>0508037025</t>
+  </si>
+  <si>
+    <t>SALEM KHALIFA SALEM RASHED</t>
   </si>
 </sst>
 </file>
@@ -207,10 +210,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -495,7 +499,7 @@
   <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,16 +626,16 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C2">
-        <v>508037025</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" t="s">
         <v>30</v>
-      </c>
-      <c r="E2" t="s">
-        <v>31</v>
       </c>
       <c r="F2" s="2">
         <v>36321</v>
@@ -640,58 +644,58 @@
         <v>24</v>
       </c>
       <c r="H2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" t="s">
         <v>32</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>33</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>34</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" t="s">
         <v>35</v>
       </c>
-      <c r="L2" t="s">
-        <v>35</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>36</v>
       </c>
-      <c r="N2" t="s">
+      <c r="R2" t="s">
         <v>37</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>38</v>
-      </c>
-      <c r="S2" t="s">
-        <v>39</v>
       </c>
       <c r="T2">
         <v>401011</v>
       </c>
       <c r="U2" t="s">
+        <v>39</v>
+      </c>
+      <c r="V2" t="s">
         <v>40</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>41</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>42</v>
-      </c>
-      <c r="X2" t="s">
-        <v>43</v>
       </c>
       <c r="Y2">
         <v>1980269076</v>
       </c>
       <c r="Z2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB2" t="s">
         <v>44</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new queues to process input data - 12/11/2025
</commit_message>
<xml_diff>
--- a/InputData.xlsx
+++ b/InputData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nirmal\Documents\UiPath\UnityBrokers_Dispatcher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B43499A-5A72-441D-AC93-8B16BABC8DF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADEC42FA-955F-4E6E-9720-1D6BA53038A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -499,7 +499,7 @@
   <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,7 +638,7 @@
         <v>30</v>
       </c>
       <c r="F2" s="2">
-        <v>36321</v>
+        <v>27030</v>
       </c>
       <c r="G2">
         <v>24</v>

</xml_diff>